<commit_message>
modified:   analysis/heat/dataqstuff/dataCollect/test.py 	modified:   analysis/heat/dataqstuff/dataCollect/thermoBoatTEC/PCR.xlsx
</commit_message>
<xml_diff>
--- a/analysis/heat/dataqstuff/dataCollect/thermoBoatTEC/PCR.xlsx
+++ b/analysis/heat/dataqstuff/dataCollect/thermoBoatTEC/PCR.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="full" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="time to temp" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="full" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="time to temp" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -151,7 +151,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <plotArea>
       <layout/>
@@ -172,14 +172,14 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -1562,14 +1562,14 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -3852,14 +3852,14 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -5560,14 +5560,14 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -6590,14 +6590,14 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -7512,14 +7512,14 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -8620,14 +8620,14 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -9206,14 +9206,14 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -9936,14 +9936,14 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -12250,14 +12250,14 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -13412,14 +13412,14 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -14472,14 +14472,14 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -17428,14 +17428,14 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -19178,14 +19178,14 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -20532,14 +20532,14 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -22372,14 +22372,14 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -23726,14 +23726,14 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -26358,14 +26358,14 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -27820,14 +27820,14 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -28832,14 +28832,14 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -30846,14 +30846,14 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -33860,9 +33860,9 @@
         <title>
           <tx>
             <rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
+              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+              <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:pPr>
                   <a:defRPr/>
                 </a:pPr>
@@ -33895,9 +33895,9 @@
         <title>
           <tx>
             <rich>
-              <a:bodyPr rot="-5400000" vert="horz"/>
-              <a:lstStyle/>
-              <a:p>
+              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="-5400000" vert="horz"/>
+              <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:pPr>
                   <a:defRPr/>
                 </a:pPr>
@@ -33930,7 +33930,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <plotArea>
       <lineChart>
@@ -33944,14 +33944,14 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -33976,14 +33976,14 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -34008,14 +34008,14 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -34040,14 +34040,14 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -34072,14 +34072,14 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -34104,14 +34104,14 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -34136,14 +34136,14 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -34168,14 +34168,14 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -34200,14 +34200,14 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -34232,14 +34232,14 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -34264,14 +34264,14 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -34296,14 +34296,14 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -34328,14 +34328,14 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -34360,14 +34360,14 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -34392,14 +34392,14 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -34424,14 +34424,14 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -34456,14 +34456,14 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -34488,14 +34488,14 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -34520,14 +34520,14 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -34552,14 +34552,14 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -34584,14 +34584,14 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln>
+              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
@@ -34643,7 +34643,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <twoCellAnchor>
     <from>
       <col>3</col>
@@ -34663,9 +34663,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -34675,7 +34675,7 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
       <col>10</col>
@@ -34690,9 +34690,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -34985,7 +34985,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -70621,12 +70621,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -70701,7 +70701,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>pass</t>
+          <t>fail</t>
         </is>
       </c>
     </row>
@@ -70800,7 +70800,7 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>pass</t>
+          <t>fail</t>
         </is>
       </c>
     </row>
@@ -70866,7 +70866,7 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>pass</t>
+          <t>fail</t>
         </is>
       </c>
     </row>
@@ -70998,7 +70998,7 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>pass</t>
+          <t>fail</t>
         </is>
       </c>
     </row>
@@ -71064,7 +71064,7 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>pass</t>
+          <t>fail</t>
         </is>
       </c>
     </row>
@@ -71097,7 +71097,7 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>pass</t>
+          <t>fail</t>
         </is>
       </c>
     </row>
@@ -71130,7 +71130,7 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>pass</t>
+          <t>fail</t>
         </is>
       </c>
     </row>
@@ -71163,7 +71163,7 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>pass</t>
+          <t>fail</t>
         </is>
       </c>
     </row>
@@ -71196,7 +71196,7 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>pass</t>
+          <t>fail</t>
         </is>
       </c>
     </row>
@@ -71229,7 +71229,7 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>pass</t>
+          <t>fail</t>
         </is>
       </c>
     </row>
@@ -71262,7 +71262,7 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>pass</t>
+          <t>fail</t>
         </is>
       </c>
     </row>
@@ -71295,7 +71295,7 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>pass</t>
+          <t>fail</t>
         </is>
       </c>
     </row>
@@ -71328,7 +71328,7 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>pass</t>
+          <t>fail</t>
         </is>
       </c>
     </row>
@@ -71361,12 +71361,12 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>pass</t>
+          <t>fail</t>
         </is>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing r:id="rId1"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>